<commit_message>
rank 1 and2 for each combination with weighted correlation result
</commit_message>
<xml_diff>
--- a/final_result.xlsx
+++ b/final_result.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>Early Morning</t>
   </si>
@@ -38,40 +38,97 @@
     <t>Saturday</t>
   </si>
   <si>
-    <t>social</t>
-  </si>
-  <si>
-    <t>Spiritual</t>
-  </si>
-  <si>
-    <t>chores</t>
-  </si>
-  <si>
-    <t>fitness</t>
+    <t>1. intellectual  2. fitness</t>
+  </si>
+  <si>
+    <t>1. physical  2. intellectual</t>
+  </si>
+  <si>
+    <t>1. physical  2. chores</t>
+  </si>
+  <si>
+    <t>1. social  2. errands</t>
+  </si>
+  <si>
+    <t>1. fitness  2. intellectual</t>
+  </si>
+  <si>
+    <t>1. chores  2. fitness</t>
   </si>
   <si>
     <t>Sunday</t>
   </si>
   <si>
-    <t>errands</t>
+    <t>1. Spiritual  2. errands</t>
+  </si>
+  <si>
+    <t>1. chores  2. errands</t>
+  </si>
+  <si>
+    <t>1. Spiritual  2. physical</t>
+  </si>
+  <si>
+    <t>1. fitness  2. physical</t>
   </si>
   <si>
     <t>Monday</t>
   </si>
   <si>
-    <t>intellectual</t>
+    <t>1. intellectual  2. physical</t>
+  </si>
+  <si>
+    <t>1. fitness  2. chores</t>
+  </si>
+  <si>
+    <t>1. social  2. fitness</t>
+  </si>
+  <si>
+    <t>1. social  2. Spiritual</t>
+  </si>
+  <si>
+    <t>1. intellectual  2. chores</t>
   </si>
   <si>
     <t>Tuesday</t>
   </si>
   <si>
+    <t>1. errands  2. fitness</t>
+  </si>
+  <si>
+    <t>1. chores  2. social</t>
+  </si>
+  <si>
+    <t>1. fitness  2. social</t>
+  </si>
+  <si>
+    <t>1. errands  2. Spiritual</t>
+  </si>
+  <si>
     <t>Wednesday</t>
   </si>
   <si>
+    <t>1. intellectual  2. errands</t>
+  </si>
+  <si>
+    <t>1. chores  2. physical</t>
+  </si>
+  <si>
+    <t>1. physical  2. fitness</t>
+  </si>
+  <si>
     <t>Thursday</t>
   </si>
   <si>
+    <t>1. errands  2. intellectual</t>
+  </si>
+  <si>
     <t>Friday</t>
+  </si>
+  <si>
+    <t>1. chores  2. Spiritual</t>
+  </si>
+  <si>
+    <t>1. intellectual  2. Spiritual</t>
   </si>
 </sst>
 </file>
@@ -462,151 +519,151 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" t="s">
         <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
         <v>9</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>9</v>
-      </c>
-      <c r="F7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>